<commit_message>
Catalog: bump version to 3
</commit_message>
<xml_diff>
--- a/input/istoki.xlsx
+++ b/input/istoki.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>